<commit_message>
The UK Case #3
</commit_message>
<xml_diff>
--- a/other-countries/data/GB/WEO_Data_Oct17_UK.xlsx
+++ b/other-countries/data/GB/WEO_Data_Oct17_UK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ayush\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB4FF7E9-0542-4B68-BAFE-D75DAD443ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5438F05B-FF70-492A-8FE3-BBDD88DBD2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3624" yWindow="2856" windowWidth="17280" windowHeight="9420" xr2:uid="{A5004343-A503-4D0E-9887-4117C87A5324}"/>
+    <workbookView xWindow="3624" yWindow="2856" windowWidth="17280" windowHeight="9420" xr2:uid="{E6C6FFC8-7F37-461C-8BD3-E486DB6FDBDD}"/>
   </bookViews>
   <sheets>
     <sheet name="WEO_Data" sheetId="1" r:id="rId1"/>
@@ -884,14 +884,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E32361-8659-49FF-BB43-84010CB434D5}">
-  <dimension ref="A1:T4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87FF2D97-0921-4114-87F7-04C7D9201383}">
+  <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -949,11 +949,17 @@
       <c r="S1">
         <v>2019</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1">
+        <v>2020</v>
+      </c>
+      <c r="U1">
+        <v>2021</v>
+      </c>
+      <c r="V1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1011,11 +1017,17 @@
       <c r="S2" s="1">
         <v>2730.6849999999999</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="1">
+        <v>2803.7849999999999</v>
+      </c>
+      <c r="U2" s="1">
+        <v>2879.777</v>
+      </c>
+      <c r="V2">
         <v>2016</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>

</xml_diff>